<commit_message>
update example excel file utk import order
</commit_message>
<xml_diff>
--- a/src/assets/file/example-import-file.xlsx
+++ b/src/assets/file/example-import-file.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="21231"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="21328"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="F:\WebHade Creative\_CLIENT\kirimin\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="F:\htdocs\kirimin\kirimin-backoffice\src\assets\file\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AA40FDA8-069F-4AA8-8612-25637558EA71}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A38A198E-444D-4240-AA32-3789553FB12A}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11310" xr2:uid="{4CDBDFBB-0F83-4B77-89A6-6066B91A26E3}"/>
   </bookViews>
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="48" uniqueCount="37">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="48" uniqueCount="38">
   <si>
     <t>Reference No.</t>
   </si>
@@ -101,9 +101,6 @@
     <t>Jawa Barat</t>
   </si>
   <si>
-    <t>Bandung</t>
-  </si>
-  <si>
     <t>pcs</t>
   </si>
   <si>
@@ -128,16 +125,22 @@
     <t>test reference 2</t>
   </si>
   <si>
-    <t>Rancasari</t>
-  </si>
-  <si>
-    <t>JL. Taman Merkuri Timur VI No.15</t>
-  </si>
-  <si>
     <t>1234567891</t>
   </si>
   <si>
-    <t>wisnu</t>
+    <t>Member</t>
+  </si>
+  <si>
+    <t>0000000001</t>
+  </si>
+  <si>
+    <t>Sukabumi</t>
+  </si>
+  <si>
+    <t>Gunung Puyuh</t>
+  </si>
+  <si>
+    <t>Alamat 1</t>
   </si>
 </sst>
 </file>
@@ -507,7 +510,7 @@
   <dimension ref="A1:U3"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A4" sqref="A4"/>
+      <selection activeCell="A3" sqref="A3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -603,7 +606,7 @@
         <v>1234567890</v>
       </c>
       <c r="B2" t="s">
-        <v>36</v>
+        <v>33</v>
       </c>
       <c r="C2" s="3" t="s">
         <v>21</v>
@@ -615,28 +618,28 @@
         <v>23</v>
       </c>
       <c r="F2" t="s">
-        <v>24</v>
+        <v>35</v>
       </c>
       <c r="G2" t="s">
-        <v>33</v>
+        <v>36</v>
       </c>
       <c r="H2" t="s">
+        <v>37</v>
+      </c>
+      <c r="I2">
+        <v>43123</v>
+      </c>
+      <c r="J2" s="3" t="s">
         <v>34</v>
-      </c>
-      <c r="I2">
-        <v>40295</v>
-      </c>
-      <c r="J2" s="3" t="s">
-        <v>21</v>
       </c>
       <c r="K2">
         <v>1</v>
       </c>
       <c r="L2" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="M2" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="N2">
         <v>1</v>
@@ -651,24 +654,24 @@
         <v>30</v>
       </c>
       <c r="R2" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="S2">
         <v>150000</v>
       </c>
       <c r="T2" t="s">
+        <v>28</v>
+      </c>
+      <c r="U2" t="s">
         <v>29</v>
-      </c>
-      <c r="U2" t="s">
-        <v>30</v>
       </c>
     </row>
     <row r="3" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A3" s="3" t="s">
-        <v>35</v>
+        <v>32</v>
       </c>
       <c r="B3" t="s">
-        <v>36</v>
+        <v>33</v>
       </c>
       <c r="C3" s="3" t="s">
         <v>21</v>
@@ -680,28 +683,28 @@
         <v>23</v>
       </c>
       <c r="F3" t="s">
-        <v>24</v>
+        <v>35</v>
       </c>
       <c r="G3" t="s">
-        <v>33</v>
+        <v>36</v>
       </c>
       <c r="H3" t="s">
+        <v>37</v>
+      </c>
+      <c r="I3">
+        <v>43123</v>
+      </c>
+      <c r="J3" s="3" t="s">
         <v>34</v>
-      </c>
-      <c r="I3">
-        <v>40295</v>
-      </c>
-      <c r="J3" s="3" t="s">
-        <v>21</v>
       </c>
       <c r="K3">
         <v>1</v>
       </c>
       <c r="L3" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="M3" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="N3">
         <v>1</v>
@@ -716,16 +719,16 @@
         <v>18</v>
       </c>
       <c r="R3" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="S3">
         <v>100000</v>
       </c>
       <c r="T3" t="s">
+        <v>30</v>
+      </c>
+      <c r="U3" t="s">
         <v>31</v>
-      </c>
-      <c r="U3" t="s">
-        <v>32</v>
       </c>
     </row>
   </sheetData>

</xml_diff>